<commit_message>
add air ship address in po
</commit_message>
<xml_diff>
--- a/results/PO_abc.xlsx
+++ b/results/PO_abc.xlsx
@@ -1512,7 +1512,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:S27"/>
+  <dimension ref="A1:S31"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="80" workbookViewId="0">
       <selection activeCell="R19" sqref="R19"/>
@@ -1757,7 +1757,11 @@
       <c r="M9" s="47" t="n"/>
       <c r="N9" s="47" t="n"/>
       <c r="O9" s="48" t="n"/>
-      <c r="P9" s="138" t="n"/>
+      <c r="P9" s="138" t="inlineStr">
+        <is>
+          <t>BCB Supply Chain Solutions</t>
+        </is>
+      </c>
       <c r="S9" s="139" t="n"/>
     </row>
     <row r="10" ht="16" customFormat="1" customHeight="1" s="25">
@@ -1777,7 +1781,11 @@
         </is>
       </c>
       <c r="O10" s="50" t="n"/>
-      <c r="P10" s="138" t="n"/>
+      <c r="P10" s="138" t="inlineStr">
+        <is>
+          <t>221 Bradgate Dr.</t>
+        </is>
+      </c>
       <c r="S10" s="139" t="n"/>
     </row>
     <row r="11" ht="16" customFormat="1" customHeight="1" s="25">
@@ -1797,7 +1805,11 @@
         </is>
       </c>
       <c r="O11" s="50" t="n"/>
-      <c r="P11" s="138" t="n"/>
+      <c r="P11" s="138" t="inlineStr">
+        <is>
+          <t>Yukon, OK 73099</t>
+        </is>
+      </c>
       <c r="S11" s="139" t="n"/>
     </row>
     <row r="12" ht="17" customFormat="1" customHeight="1" s="25" thickBot="1">
@@ -2124,236 +2136,412 @@
       </c>
     </row>
     <row r="18" ht="20" customHeight="1">
-      <c r="B18" s="154" t="inlineStr">
+      <c r="B18" s="149" t="inlineStr">
         <is>
           <t>1</t>
         </is>
       </c>
-      <c r="C18" s="155" t="n">
+      <c r="C18" s="150" t="n">
         <v>1000</v>
       </c>
-      <c r="D18" s="156" t="n"/>
-      <c r="E18" s="155" t="inlineStr">
+      <c r="D18" s="151" t="n"/>
+      <c r="E18" s="150" t="inlineStr">
         <is>
           <t>22002</t>
         </is>
       </c>
-      <c r="F18" s="155" t="inlineStr"/>
-      <c r="G18" s="155" t="inlineStr"/>
-      <c r="H18" s="156" t="n"/>
-      <c r="I18" s="156" t="n"/>
-      <c r="J18" s="155" t="inlineStr"/>
-      <c r="K18" s="155" t="inlineStr">
+      <c r="F18" s="150" t="inlineStr"/>
+      <c r="G18" s="150" t="inlineStr"/>
+      <c r="H18" s="151" t="n"/>
+      <c r="I18" s="151" t="n"/>
+      <c r="J18" s="150" t="inlineStr"/>
+      <c r="K18" s="150" t="inlineStr">
         <is>
           <t>DI</t>
         </is>
       </c>
-      <c r="L18" s="155" t="inlineStr">
+      <c r="L18" s="150" t="inlineStr">
         <is>
           <t>Sea</t>
         </is>
       </c>
-      <c r="M18" s="157" t="n">
+      <c r="M18" s="152" t="n">
         <v>45531</v>
       </c>
-      <c r="N18" s="155" t="n"/>
-      <c r="O18" s="155" t="n"/>
-      <c r="P18" s="156" t="n"/>
-      <c r="Q18" s="155" t="n">
+      <c r="N18" s="150" t="n"/>
+      <c r="O18" s="150" t="n"/>
+      <c r="P18" s="151" t="n"/>
+      <c r="Q18" s="150" t="n">
         <v>13.26</v>
       </c>
-      <c r="R18" s="156" t="n"/>
-      <c r="S18" s="158" t="n">
+      <c r="R18" s="151" t="n"/>
+      <c r="S18" s="153" t="n">
         <v>13260</v>
       </c>
     </row>
-    <row r="19" ht="16" customHeight="1" thickBot="1">
-      <c r="B19" s="13" t="n"/>
-      <c r="C19" s="14" t="n"/>
-      <c r="D19" s="9" t="n"/>
-      <c r="E19" s="15" t="n"/>
-      <c r="F19" s="15" t="n"/>
-      <c r="G19" s="8" t="n"/>
-      <c r="H19" s="8" t="n"/>
-      <c r="I19" s="8" t="n"/>
-      <c r="J19" s="10" t="n"/>
-      <c r="K19" s="101" t="n"/>
-      <c r="L19" s="9" t="n"/>
-      <c r="M19" s="159" t="n"/>
-      <c r="N19" s="159" t="n"/>
-      <c r="O19" s="31" t="n"/>
-      <c r="P19" s="160" t="n"/>
-      <c r="Q19" s="160" t="n"/>
-      <c r="R19" s="160" t="n"/>
-      <c r="S19" s="161" t="n"/>
-    </row>
-    <row r="20" ht="16" customHeight="1" thickTop="1">
-      <c r="B20" s="13" t="n"/>
-      <c r="C20" s="14" t="n"/>
-      <c r="D20" s="9" t="n"/>
-      <c r="E20" s="15" t="n"/>
-      <c r="F20" s="15" t="n"/>
-      <c r="G20" s="8" t="n"/>
-      <c r="H20" s="8" t="n"/>
-      <c r="I20" s="8" t="n"/>
-      <c r="J20" s="10" t="n"/>
-      <c r="K20" s="101" t="n"/>
-      <c r="L20" s="9" t="n"/>
-      <c r="M20" s="159" t="n"/>
-      <c r="N20" s="159" t="n"/>
-      <c r="O20" s="31" t="n"/>
-      <c r="P20" s="160" t="n"/>
-      <c r="Q20" s="160" t="n"/>
-      <c r="R20" s="160" t="n"/>
-      <c r="S20" s="161" t="n"/>
-    </row>
-    <row r="21">
-      <c r="M21" s="17" t="n"/>
-      <c r="N21" s="33" t="n"/>
-      <c r="O21" s="33" t="n"/>
-      <c r="P21" s="79" t="inlineStr">
+    <row r="19" ht="20" customHeight="1" thickBot="1">
+      <c r="B19" s="149" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="C19" s="150" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D19" s="151" t="n"/>
+      <c r="E19" s="150" t="inlineStr">
+        <is>
+          <t>22002</t>
+        </is>
+      </c>
+      <c r="F19" s="150" t="inlineStr"/>
+      <c r="G19" s="150" t="inlineStr"/>
+      <c r="H19" s="151" t="n"/>
+      <c r="I19" s="151" t="n"/>
+      <c r="J19" s="150" t="inlineStr"/>
+      <c r="K19" s="150" t="inlineStr">
+        <is>
+          <t>DI</t>
+        </is>
+      </c>
+      <c r="L19" s="150" t="inlineStr">
+        <is>
+          <t>Sea</t>
+        </is>
+      </c>
+      <c r="M19" s="152" t="n">
+        <v>45531</v>
+      </c>
+      <c r="N19" s="150" t="n"/>
+      <c r="O19" s="150" t="n"/>
+      <c r="P19" s="151" t="n"/>
+      <c r="Q19" s="150" t="n">
+        <v>13.26</v>
+      </c>
+      <c r="R19" s="151" t="n"/>
+      <c r="S19" s="153" t="n">
+        <v>13260</v>
+      </c>
+    </row>
+    <row r="20" ht="20" customHeight="1" thickTop="1">
+      <c r="B20" s="149" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="C20" s="150" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D20" s="151" t="n"/>
+      <c r="E20" s="150" t="inlineStr">
+        <is>
+          <t>22002</t>
+        </is>
+      </c>
+      <c r="F20" s="150" t="inlineStr"/>
+      <c r="G20" s="150" t="inlineStr"/>
+      <c r="H20" s="151" t="n"/>
+      <c r="I20" s="151" t="n"/>
+      <c r="J20" s="150" t="inlineStr"/>
+      <c r="K20" s="150" t="inlineStr">
+        <is>
+          <t>DI</t>
+        </is>
+      </c>
+      <c r="L20" s="150" t="inlineStr">
+        <is>
+          <t>Sea</t>
+        </is>
+      </c>
+      <c r="M20" s="152" t="n">
+        <v>45531</v>
+      </c>
+      <c r="N20" s="150" t="n"/>
+      <c r="O20" s="150" t="n"/>
+      <c r="P20" s="151" t="n"/>
+      <c r="Q20" s="150" t="n">
+        <v>13.26</v>
+      </c>
+      <c r="R20" s="151" t="n"/>
+      <c r="S20" s="153" t="n">
+        <v>13260</v>
+      </c>
+    </row>
+    <row r="21" ht="20" customHeight="1">
+      <c r="B21" s="149" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="C21" s="150" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D21" s="151" t="n"/>
+      <c r="E21" s="150" t="inlineStr">
+        <is>
+          <t>22002</t>
+        </is>
+      </c>
+      <c r="F21" s="150" t="inlineStr"/>
+      <c r="G21" s="150" t="inlineStr"/>
+      <c r="H21" s="151" t="n"/>
+      <c r="I21" s="151" t="n"/>
+      <c r="J21" s="150" t="inlineStr"/>
+      <c r="K21" s="150" t="inlineStr">
+        <is>
+          <t>DI</t>
+        </is>
+      </c>
+      <c r="L21" s="150" t="inlineStr">
+        <is>
+          <t>Sea</t>
+        </is>
+      </c>
+      <c r="M21" s="152" t="n">
+        <v>45531</v>
+      </c>
+      <c r="N21" s="150" t="n"/>
+      <c r="O21" s="150" t="n"/>
+      <c r="P21" s="151" t="n"/>
+      <c r="Q21" s="150" t="n">
+        <v>13.26</v>
+      </c>
+      <c r="R21" s="151" t="n"/>
+      <c r="S21" s="153" t="n">
+        <v>13260</v>
+      </c>
+    </row>
+    <row r="22" ht="20" customHeight="1">
+      <c r="B22" s="154" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="C22" s="155" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D22" s="156" t="n"/>
+      <c r="E22" s="155" t="inlineStr">
+        <is>
+          <t>22002</t>
+        </is>
+      </c>
+      <c r="F22" s="155" t="inlineStr"/>
+      <c r="G22" s="155" t="inlineStr"/>
+      <c r="H22" s="156" t="n"/>
+      <c r="I22" s="156" t="n"/>
+      <c r="J22" s="155" t="inlineStr"/>
+      <c r="K22" s="155" t="inlineStr">
+        <is>
+          <t>DI</t>
+        </is>
+      </c>
+      <c r="L22" s="155" t="inlineStr">
+        <is>
+          <t>Sea</t>
+        </is>
+      </c>
+      <c r="M22" s="157" t="n">
+        <v>45531</v>
+      </c>
+      <c r="N22" s="155" t="n"/>
+      <c r="O22" s="155" t="n"/>
+      <c r="P22" s="156" t="n"/>
+      <c r="Q22" s="155" t="n">
+        <v>13.26</v>
+      </c>
+      <c r="R22" s="156" t="n"/>
+      <c r="S22" s="158" t="n">
+        <v>13260</v>
+      </c>
+    </row>
+    <row r="23" ht="14" customFormat="1" customHeight="1" s="2" thickBot="1">
+      <c r="B23" s="13" t="n"/>
+      <c r="C23" s="14" t="n"/>
+      <c r="D23" s="9" t="n"/>
+      <c r="E23" s="15" t="n"/>
+      <c r="F23" s="15" t="n"/>
+      <c r="G23" s="8" t="n"/>
+      <c r="H23" s="8" t="n"/>
+      <c r="I23" s="8" t="n"/>
+      <c r="J23" s="10" t="n"/>
+      <c r="K23" s="101" t="n"/>
+      <c r="L23" s="9" t="n"/>
+      <c r="M23" s="159" t="n"/>
+      <c r="N23" s="159" t="n"/>
+      <c r="O23" s="31" t="n"/>
+      <c r="P23" s="160" t="n"/>
+      <c r="Q23" s="160" t="n"/>
+      <c r="R23" s="160" t="n"/>
+      <c r="S23" s="161" t="n"/>
+    </row>
+    <row r="24" ht="16" customFormat="1" customHeight="1" s="2">
+      <c r="B24" s="13" t="n"/>
+      <c r="C24" s="14" t="n"/>
+      <c r="D24" s="9" t="n"/>
+      <c r="E24" s="15" t="n"/>
+      <c r="F24" s="15" t="n"/>
+      <c r="G24" s="8" t="n"/>
+      <c r="H24" s="8" t="n"/>
+      <c r="I24" s="8" t="n"/>
+      <c r="J24" s="10" t="n"/>
+      <c r="K24" s="101" t="n"/>
+      <c r="L24" s="9" t="n"/>
+      <c r="M24" s="159" t="n"/>
+      <c r="N24" s="159" t="n"/>
+      <c r="O24" s="31" t="n"/>
+      <c r="P24" s="160" t="n"/>
+      <c r="Q24" s="160" t="n"/>
+      <c r="R24" s="160" t="n"/>
+      <c r="S24" s="161" t="n"/>
+    </row>
+    <row r="25" ht="14" customHeight="1">
+      <c r="M25" s="17" t="n"/>
+      <c r="N25" s="33" t="n"/>
+      <c r="O25" s="33" t="n"/>
+      <c r="P25" s="79" t="inlineStr">
         <is>
           <t>合计</t>
         </is>
       </c>
-      <c r="Q21" s="36" t="inlineStr">
+      <c r="Q25" s="36" t="inlineStr">
         <is>
           <t>( TOTAL)</t>
         </is>
       </c>
-      <c r="R21" s="162" t="n">
-        <v>26520</v>
-      </c>
-      <c r="S21" s="117" t="n"/>
-    </row>
-    <row r="22" ht="14" customHeight="1">
-      <c r="B22" s="85" t="inlineStr">
+      <c r="R25" s="162" t="n">
+        <v>79560</v>
+      </c>
+      <c r="S25" s="117" t="n"/>
+    </row>
+    <row r="26">
+      <c r="B26" s="85" t="inlineStr">
         <is>
           <t>说明（NOTE）:</t>
         </is>
       </c>
-      <c r="C22" s="86" t="n"/>
-      <c r="D22" s="86" t="n"/>
-      <c r="E22" s="86" t="n"/>
-      <c r="F22" s="87" t="n"/>
-      <c r="G22" s="87" t="n"/>
-      <c r="H22" s="87" t="n"/>
-      <c r="I22" s="87" t="n"/>
-      <c r="J22" s="88" t="n"/>
-      <c r="K22" s="102" t="n"/>
-      <c r="L22" s="89" t="n"/>
-      <c r="M22" s="90" t="n"/>
-      <c r="N22" s="33" t="n"/>
-      <c r="O22" s="33" t="n"/>
-      <c r="P22" s="163" t="n"/>
-      <c r="Q22" s="43" t="n"/>
-      <c r="R22" s="43" t="n"/>
-      <c r="S22" s="44" t="n"/>
-    </row>
-    <row r="23" ht="14" customFormat="1" customHeight="1" s="2" thickBot="1">
-      <c r="B23" s="110" t="n"/>
-      <c r="C23" s="111" t="n"/>
-      <c r="D23" s="111" t="n"/>
-      <c r="E23" s="111" t="n"/>
-      <c r="F23" s="111" t="n"/>
-      <c r="G23" s="111" t="n"/>
-      <c r="H23" s="111" t="n"/>
-      <c r="I23" s="111" t="n"/>
-      <c r="J23" s="111" t="n"/>
-      <c r="K23" s="111" t="n"/>
-      <c r="L23" s="111" t="n"/>
-      <c r="M23" s="112" t="n"/>
-    </row>
-    <row r="24" ht="16" customFormat="1" customHeight="1" s="2">
-      <c r="B24" s="110" t="n"/>
-      <c r="C24" s="111" t="n"/>
-      <c r="D24" s="111" t="n"/>
-      <c r="E24" s="111" t="n"/>
-      <c r="F24" s="111" t="n"/>
-      <c r="G24" s="111" t="n"/>
-      <c r="H24" s="111" t="n"/>
-      <c r="I24" s="111" t="n"/>
-      <c r="J24" s="111" t="n"/>
-      <c r="K24" s="111" t="n"/>
-      <c r="L24" s="111" t="n"/>
-      <c r="M24" s="112" t="n"/>
-      <c r="P24" s="83" t="inlineStr">
+      <c r="C26" s="86" t="n"/>
+      <c r="D26" s="86" t="n"/>
+      <c r="E26" s="86" t="n"/>
+      <c r="F26" s="87" t="n"/>
+      <c r="G26" s="87" t="n"/>
+      <c r="H26" s="87" t="n"/>
+      <c r="I26" s="87" t="n"/>
+      <c r="J26" s="88" t="n"/>
+      <c r="K26" s="102" t="n"/>
+      <c r="L26" s="89" t="n"/>
+      <c r="M26" s="90" t="n"/>
+      <c r="N26" s="33" t="n"/>
+      <c r="O26" s="33" t="n"/>
+      <c r="P26" s="163" t="n"/>
+      <c r="Q26" s="43" t="n"/>
+      <c r="R26" s="43" t="n"/>
+      <c r="S26" s="44" t="n"/>
+    </row>
+    <row r="27">
+      <c r="B27" s="110" t="n"/>
+      <c r="C27" s="111" t="n"/>
+      <c r="D27" s="111" t="n"/>
+      <c r="E27" s="111" t="n"/>
+      <c r="F27" s="111" t="n"/>
+      <c r="G27" s="111" t="n"/>
+      <c r="H27" s="111" t="n"/>
+      <c r="I27" s="111" t="n"/>
+      <c r="J27" s="111" t="n"/>
+      <c r="K27" s="111" t="n"/>
+      <c r="L27" s="111" t="n"/>
+      <c r="M27" s="112" t="n"/>
+    </row>
+    <row r="28">
+      <c r="B28" s="110" t="n"/>
+      <c r="C28" s="111" t="n"/>
+      <c r="D28" s="111" t="n"/>
+      <c r="E28" s="111" t="n"/>
+      <c r="F28" s="111" t="n"/>
+      <c r="G28" s="111" t="n"/>
+      <c r="H28" s="111" t="n"/>
+      <c r="I28" s="111" t="n"/>
+      <c r="J28" s="111" t="n"/>
+      <c r="K28" s="111" t="n"/>
+      <c r="L28" s="111" t="n"/>
+      <c r="M28" s="112" t="n"/>
+      <c r="P28" s="83" t="inlineStr">
         <is>
           <t>订单签发人 (BY):</t>
         </is>
       </c>
-      <c r="Q24" s="164" t="n"/>
-      <c r="R24" s="165" t="inlineStr">
+      <c r="Q28" s="164" t="n"/>
+      <c r="R28" s="165" t="inlineStr">
         <is>
           <t>Tim Qi</t>
         </is>
       </c>
     </row>
-    <row r="25" ht="14" customHeight="1">
-      <c r="B25" s="113" t="n"/>
-      <c r="C25" s="114" t="n"/>
-      <c r="D25" s="114" t="n"/>
-      <c r="E25" s="114" t="n"/>
-      <c r="F25" s="114" t="n"/>
-      <c r="G25" s="114" t="n"/>
-      <c r="H25" s="114" t="n"/>
-      <c r="I25" s="114" t="n"/>
-      <c r="J25" s="114" t="n"/>
-      <c r="K25" s="114" t="n"/>
-      <c r="L25" s="114" t="n"/>
-      <c r="M25" s="115" t="n"/>
-      <c r="N25" s="19" t="n"/>
-      <c r="O25" s="19" t="n"/>
-      <c r="Q25" s="166" t="n"/>
-      <c r="R25" s="167" t="n"/>
-      <c r="S25" s="168" t="n"/>
-    </row>
-    <row r="26">
-      <c r="B26" s="4" t="n"/>
-      <c r="C26" s="4" t="n"/>
-      <c r="D26" s="4" t="n"/>
-      <c r="E26" s="4" t="n"/>
-      <c r="F26" s="24" t="n"/>
-      <c r="G26" s="24" t="n"/>
-      <c r="H26" s="24" t="n"/>
-      <c r="I26" s="24" t="n"/>
-      <c r="J26" s="4" t="n"/>
-      <c r="K26" s="103" t="n"/>
-      <c r="L26" s="18" t="n"/>
-      <c r="M26" s="18" t="n"/>
-      <c r="N26" s="18" t="n"/>
-      <c r="O26" s="18" t="n"/>
-      <c r="P26" s="4" t="n"/>
-      <c r="Q26" s="169" t="n"/>
-      <c r="R26" s="169" t="n"/>
-      <c r="S26" s="170" t="n"/>
-    </row>
-    <row r="27">
-      <c r="B27" s="19" t="inlineStr">
+    <row r="29">
+      <c r="B29" s="113" t="n"/>
+      <c r="C29" s="114" t="n"/>
+      <c r="D29" s="114" t="n"/>
+      <c r="E29" s="114" t="n"/>
+      <c r="F29" s="114" t="n"/>
+      <c r="G29" s="114" t="n"/>
+      <c r="H29" s="114" t="n"/>
+      <c r="I29" s="114" t="n"/>
+      <c r="J29" s="114" t="n"/>
+      <c r="K29" s="114" t="n"/>
+      <c r="L29" s="114" t="n"/>
+      <c r="M29" s="115" t="n"/>
+      <c r="N29" s="19" t="n"/>
+      <c r="O29" s="19" t="n"/>
+      <c r="Q29" s="166" t="n"/>
+      <c r="R29" s="167" t="n"/>
+      <c r="S29" s="168" t="n"/>
+    </row>
+    <row r="30">
+      <c r="B30" s="4" t="n"/>
+      <c r="C30" s="4" t="n"/>
+      <c r="D30" s="4" t="n"/>
+      <c r="E30" s="4" t="n"/>
+      <c r="F30" s="24" t="n"/>
+      <c r="G30" s="24" t="n"/>
+      <c r="H30" s="24" t="n"/>
+      <c r="I30" s="24" t="n"/>
+      <c r="J30" s="4" t="n"/>
+      <c r="K30" s="103" t="n"/>
+      <c r="L30" s="18" t="n"/>
+      <c r="M30" s="18" t="n"/>
+      <c r="N30" s="18" t="n"/>
+      <c r="O30" s="18" t="n"/>
+      <c r="P30" s="4" t="n"/>
+      <c r="Q30" s="169" t="n"/>
+      <c r="R30" s="169" t="n"/>
+      <c r="S30" s="170" t="n"/>
+    </row>
+    <row r="31">
+      <c r="B31" s="19" t="inlineStr">
         <is>
           <t xml:space="preserve">    Please notify us immediately if you are unable to deliver as specified.</t>
         </is>
       </c>
-      <c r="C27" s="4" t="n"/>
-      <c r="D27" s="4" t="n"/>
-      <c r="E27" s="4" t="n"/>
-      <c r="F27" s="24" t="n"/>
-      <c r="G27" s="24" t="n"/>
-      <c r="H27" s="24" t="n"/>
-      <c r="I27" s="24" t="n"/>
-      <c r="J27" s="4" t="n"/>
-      <c r="K27" s="104" t="n"/>
-      <c r="L27" s="4" t="n"/>
-      <c r="P27" s="171" t="inlineStr">
+      <c r="C31" s="4" t="n"/>
+      <c r="D31" s="4" t="n"/>
+      <c r="E31" s="4" t="n"/>
+      <c r="F31" s="24" t="n"/>
+      <c r="G31" s="24" t="n"/>
+      <c r="H31" s="24" t="n"/>
+      <c r="I31" s="24" t="n"/>
+      <c r="J31" s="4" t="n"/>
+      <c r="K31" s="104" t="n"/>
+      <c r="L31" s="4" t="n"/>
+      <c r="P31" s="171" t="inlineStr">
         <is>
           <t>订货日期 (ORDER DATE):</t>
         </is>
       </c>
-      <c r="Q27" s="165" t="n"/>
-      <c r="R27" s="172" t="n">
+      <c r="Q31" s="165" t="n"/>
+      <c r="R31" s="172" t="n">
         <v>45533</v>
       </c>
-      <c r="S27" s="172" t="n"/>
+      <c r="S31" s="172" t="n"/>
     </row>
   </sheetData>
   <mergeCells count="11">

</xml_diff>